<commit_message>
Adding docs to the analysis tools module
</commit_message>
<xml_diff>
--- a/data/raw/Running.xlsx
+++ b/data/raw/Running.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Running\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F558134-4578-459C-A574-385E30E85817}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{008AA7FB-5EB6-4181-AA61-712EBC8FB378}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" xr2:uid="{A2ECB18D-D6A8-48F0-BC89-850EAC9BB528}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A2ECB18D-D6A8-48F0-BC89-850EAC9BB528}"/>
   </bookViews>
   <sheets>
     <sheet name="Runs" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="329">
   <si>
     <t>Date</t>
   </si>
@@ -1615,7 +1615,7 @@
   <dimension ref="A1:W201"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A193" zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
-      <selection activeCell="D198" sqref="D198"/>
+      <selection activeCell="F210" sqref="F210"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25.8" outlineLevelCol="1" x14ac:dyDescent="0.5"/>
@@ -10956,81 +10956,97 @@
       </c>
     </row>
     <row r="198" spans="1:23" x14ac:dyDescent="0.5">
-      <c r="A198" s="4"/>
-      <c r="B198" s="2"/>
-      <c r="C198" s="2"/>
-      <c r="D198" s="5"/>
+      <c r="A198" s="4">
+        <v>44326</v>
+      </c>
+      <c r="B198" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C198" s="2">
+        <v>12150</v>
+      </c>
+      <c r="D198" s="5">
+        <v>84.23</v>
+      </c>
       <c r="E198" s="2">
         <f>SUM($C$2:C198)</f>
-        <v>1661900</v>
+        <v>1674050</v>
       </c>
       <c r="F198" s="5">
         <f>SUM($T$2:T198) + V198 + W198</f>
-        <v>9419.3799999999992</v>
+        <v>9504.01</v>
       </c>
       <c r="G198" s="5">
         <f t="shared" si="24"/>
-        <v>156.98966666666666</v>
+        <v>158.40016666666668</v>
       </c>
       <c r="H198" s="10">
         <f t="shared" si="25"/>
-        <v>1.5698966666666665</v>
+        <v>1.5840016666666668</v>
       </c>
       <c r="I198" s="10"/>
       <c r="T198" s="1">
         <f t="shared" si="26"/>
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="U198" s="1">
         <f t="shared" si="27"/>
-        <v>0</v>
+        <v>23.000000000000398</v>
       </c>
       <c r="V198">
         <f>INT(SUM($U$2:U198)/60)</f>
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="W198">
         <f>(SUM($U$2:U198)-60*V198)/100</f>
-        <v>0.3799999999999909</v>
+        <v>9.9999999999954518E-3</v>
       </c>
     </row>
     <row r="199" spans="1:23" x14ac:dyDescent="0.5">
-      <c r="A199" s="4"/>
-      <c r="B199" s="2"/>
-      <c r="C199" s="2"/>
-      <c r="D199" s="5"/>
+      <c r="A199" s="4">
+        <v>44327</v>
+      </c>
+      <c r="B199" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C199" s="2">
+        <v>60004</v>
+      </c>
+      <c r="D199" s="5">
+        <v>33.56</v>
+      </c>
       <c r="E199" s="2">
         <f>SUM($C$2:C199)</f>
-        <v>1661900</v>
+        <v>1734054</v>
       </c>
       <c r="F199" s="5">
         <f>SUM($T$2:T199) + V199 + W199</f>
-        <v>9419.3799999999992</v>
+        <v>9537.57</v>
       </c>
       <c r="G199" s="5">
         <f t="shared" si="24"/>
-        <v>156.98966666666666</v>
+        <v>158.95949999999999</v>
       </c>
       <c r="H199" s="10">
         <f t="shared" si="25"/>
-        <v>1.5698966666666665</v>
+        <v>1.5895949999999999</v>
       </c>
       <c r="I199" s="10"/>
       <c r="T199" s="1">
         <f t="shared" si="26"/>
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="U199" s="1">
         <f t="shared" si="27"/>
-        <v>0</v>
+        <v>56.000000000000227</v>
       </c>
       <c r="V199">
         <f>INT(SUM($U$2:U199)/60)</f>
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="W199">
         <f>(SUM($U$2:U199)-60*V199)/100</f>
-        <v>0.3799999999999909</v>
+        <v>0.56999999999999995</v>
       </c>
     </row>
     <row r="200" spans="1:23" x14ac:dyDescent="0.5">
@@ -11040,19 +11056,19 @@
       <c r="D200" s="5"/>
       <c r="E200" s="2">
         <f>SUM($C$2:C200)</f>
-        <v>1661900</v>
+        <v>1734054</v>
       </c>
       <c r="F200" s="5">
         <f>SUM($T$2:T200) + V200 + W200</f>
-        <v>9419.3799999999992</v>
+        <v>9537.57</v>
       </c>
       <c r="G200" s="5">
         <f t="shared" si="24"/>
-        <v>156.98966666666666</v>
+        <v>158.95949999999999</v>
       </c>
       <c r="H200" s="10">
         <f t="shared" si="25"/>
-        <v>1.5698966666666665</v>
+        <v>1.5895949999999999</v>
       </c>
       <c r="I200" s="10"/>
       <c r="T200" s="1">
@@ -11065,11 +11081,11 @@
       </c>
       <c r="V200">
         <f>INT(SUM($U$2:U200)/60)</f>
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="W200">
         <f>(SUM($U$2:U200)-60*V200)/100</f>
-        <v>0.3799999999999909</v>
+        <v>0.56999999999999995</v>
       </c>
     </row>
     <row r="201" spans="1:23" x14ac:dyDescent="0.5">
@@ -11079,19 +11095,19 @@
       <c r="D201" s="5"/>
       <c r="E201" s="2">
         <f>SUM($C$2:C201)</f>
-        <v>1661900</v>
+        <v>1734054</v>
       </c>
       <c r="F201" s="5">
         <f>SUM($T$2:T201) + V201 + W201</f>
-        <v>9419.3799999999992</v>
+        <v>9537.57</v>
       </c>
       <c r="G201" s="5">
         <f t="shared" si="24"/>
-        <v>156.98966666666666</v>
+        <v>158.95949999999999</v>
       </c>
       <c r="H201" s="10">
         <f t="shared" si="25"/>
-        <v>1.5698966666666665</v>
+        <v>1.5895949999999999</v>
       </c>
       <c r="I201" s="10"/>
       <c r="T201" s="1">
@@ -11104,11 +11120,11 @@
       </c>
       <c r="V201">
         <f>INT(SUM($U$2:U201)/60)</f>
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="W201">
         <f>(SUM($U$2:U201)-60*V201)/100</f>
-        <v>0.3799999999999909</v>
+        <v>0.56999999999999995</v>
       </c>
     </row>
   </sheetData>
@@ -28640,21 +28656,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100752C5226F4F40D4984F6AAC1D14871F4" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="efe049bb4e45d5e2f6191c883107bca1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c63f97c9-a388-4650-84b1-91345983bc9a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="298f3f6395e194b72b5b7a1e46caeb33" ns3:_="">
     <xsd:import namespace="c63f97c9-a388-4650-84b1-91345983bc9a"/>
@@ -28786,10 +28787,35 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CEEE6BA5-4888-413F-968E-F29225E87763}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6DD7B093-18AC-4B9F-AB72-EEF4E212A659}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="c63f97c9-a388-4650-84b1-91345983bc9a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -28811,19 +28837,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6DD7B093-18AC-4B9F-AB72-EEF4E212A659}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CEEE6BA5-4888-413F-968E-F29225E87763}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="c63f97c9-a388-4650-84b1-91345983bc9a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Adding docs to read and merge
</commit_message>
<xml_diff>
--- a/data/raw/Running.xlsx
+++ b/data/raw/Running.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Running\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{008AA7FB-5EB6-4181-AA61-712EBC8FB378}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B000F795-7941-434B-BBE2-8C8D84E8A68A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A2ECB18D-D6A8-48F0-BC89-850EAC9BB528}"/>
+    <workbookView xWindow="28680" yWindow="-2220" windowWidth="15600" windowHeight="11160" xr2:uid="{A2ECB18D-D6A8-48F0-BC89-850EAC9BB528}"/>
   </bookViews>
   <sheets>
     <sheet name="Runs" sheetId="1" r:id="rId1"/>
@@ -1614,8 +1614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AD3663A-1B36-42F8-92D9-0C097A8D0EBA}">
   <dimension ref="A1:W201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A193" zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
-      <selection activeCell="F210" sqref="F210"/>
+    <sheetView tabSelected="1" topLeftCell="A187" zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
+      <selection activeCell="B201" sqref="B201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25.8" outlineLevelCol="1" x14ac:dyDescent="0.5"/>
@@ -28656,6 +28656,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100752C5226F4F40D4984F6AAC1D14871F4" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="efe049bb4e45d5e2f6191c883107bca1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c63f97c9-a388-4650-84b1-91345983bc9a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="298f3f6395e194b72b5b7a1e46caeb33" ns3:_="">
     <xsd:import namespace="c63f97c9-a388-4650-84b1-91345983bc9a"/>
@@ -28787,35 +28802,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6DD7B093-18AC-4B9F-AB72-EEF4E212A659}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CEEE6BA5-4888-413F-968E-F29225E87763}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="c63f97c9-a388-4650-84b1-91345983bc9a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -28837,9 +28827,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CEEE6BA5-4888-413F-968E-F29225E87763}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6DD7B093-18AC-4B9F-AB72-EEF4E212A659}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="c63f97c9-a388-4650-84b1-91345983bc9a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Adding to Scripts read and merge docs
</commit_message>
<xml_diff>
--- a/data/raw/Running.xlsx
+++ b/data/raw/Running.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Running\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B000F795-7941-434B-BBE2-8C8D84E8A68A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA5A68F3-003F-42EB-BDAA-C5A7F0B20777}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-2220" windowWidth="15600" windowHeight="11160" xr2:uid="{A2ECB18D-D6A8-48F0-BC89-850EAC9BB528}"/>
   </bookViews>
@@ -1615,7 +1615,7 @@
   <dimension ref="A1:W201"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A187" zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
-      <selection activeCell="B201" sqref="B201"/>
+      <selection activeCell="D204" sqref="D204"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25.8" outlineLevelCol="1" x14ac:dyDescent="0.5"/>
@@ -11010,14 +11010,14 @@
         <v>7</v>
       </c>
       <c r="C199" s="2">
-        <v>60004</v>
+        <v>6004</v>
       </c>
       <c r="D199" s="5">
         <v>33.56</v>
       </c>
       <c r="E199" s="2">
         <f>SUM($C$2:C199)</f>
-        <v>1734054</v>
+        <v>1680054</v>
       </c>
       <c r="F199" s="5">
         <f>SUM($T$2:T199) + V199 + W199</f>
@@ -11056,7 +11056,7 @@
       <c r="D200" s="5"/>
       <c r="E200" s="2">
         <f>SUM($C$2:C200)</f>
-        <v>1734054</v>
+        <v>1680054</v>
       </c>
       <c r="F200" s="5">
         <f>SUM($T$2:T200) + V200 + W200</f>
@@ -11095,7 +11095,7 @@
       <c r="D201" s="5"/>
       <c r="E201" s="2">
         <f>SUM($C$2:C201)</f>
-        <v>1734054</v>
+        <v>1680054</v>
       </c>
       <c r="F201" s="5">
         <f>SUM($T$2:T201) + V201 + W201</f>

</xml_diff>

<commit_message>
Adding new goal chart
</commit_message>
<xml_diff>
--- a/data/raw/Running.xlsx
+++ b/data/raw/Running.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Running\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA5A68F3-003F-42EB-BDAA-C5A7F0B20777}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D148B7C9-F778-45F5-BCEF-E680189D8CC7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-2220" windowWidth="15600" windowHeight="11160" xr2:uid="{A2ECB18D-D6A8-48F0-BC89-850EAC9BB528}"/>
+    <workbookView xWindow="1524" yWindow="0" windowWidth="17280" windowHeight="8964" xr2:uid="{A2ECB18D-D6A8-48F0-BC89-850EAC9BB528}"/>
   </bookViews>
   <sheets>
     <sheet name="Runs" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="329">
   <si>
     <t>Date</t>
   </si>
@@ -1614,8 +1614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AD3663A-1B36-42F8-92D9-0C097A8D0EBA}">
   <dimension ref="A1:W201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A187" zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
-      <selection activeCell="D204" sqref="D204"/>
+    <sheetView tabSelected="1" topLeftCell="A189" zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
+      <selection activeCell="E199" sqref="E199"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25.8" outlineLevelCol="1" x14ac:dyDescent="0.5"/>
@@ -11050,42 +11050,50 @@
       </c>
     </row>
     <row r="200" spans="1:23" x14ac:dyDescent="0.5">
-      <c r="A200" s="4"/>
-      <c r="B200" s="2"/>
-      <c r="C200" s="2"/>
-      <c r="D200" s="5"/>
+      <c r="A200" s="4">
+        <v>44329</v>
+      </c>
+      <c r="B200" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C200" s="2">
+        <v>10210</v>
+      </c>
+      <c r="D200" s="5">
+        <v>59.35</v>
+      </c>
       <c r="E200" s="2">
         <f>SUM($C$2:C200)</f>
-        <v>1680054</v>
+        <v>1690264</v>
       </c>
       <c r="F200" s="5">
         <f>SUM($T$2:T200) + V200 + W200</f>
-        <v>9537.57</v>
+        <v>9597.32</v>
       </c>
       <c r="G200" s="5">
         <f t="shared" si="24"/>
-        <v>158.95949999999999</v>
+        <v>159.95533333333333</v>
       </c>
       <c r="H200" s="10">
         <f t="shared" si="25"/>
-        <v>1.5895949999999999</v>
+        <v>1.5995533333333332</v>
       </c>
       <c r="I200" s="10"/>
       <c r="T200" s="1">
         <f t="shared" si="26"/>
-        <v>0</v>
+        <v>59</v>
       </c>
       <c r="U200" s="1">
         <f t="shared" si="27"/>
-        <v>0</v>
+        <v>35.000000000000142</v>
       </c>
       <c r="V200">
         <f>INT(SUM($U$2:U200)/60)</f>
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="W200">
         <f>(SUM($U$2:U200)-60*V200)/100</f>
-        <v>0.56999999999999995</v>
+        <v>0.32</v>
       </c>
     </row>
     <row r="201" spans="1:23" x14ac:dyDescent="0.5">
@@ -11095,19 +11103,19 @@
       <c r="D201" s="5"/>
       <c r="E201" s="2">
         <f>SUM($C$2:C201)</f>
-        <v>1680054</v>
+        <v>1690264</v>
       </c>
       <c r="F201" s="5">
         <f>SUM($T$2:T201) + V201 + W201</f>
-        <v>9537.57</v>
+        <v>9597.32</v>
       </c>
       <c r="G201" s="5">
         <f t="shared" si="24"/>
-        <v>158.95949999999999</v>
+        <v>159.95533333333333</v>
       </c>
       <c r="H201" s="10">
         <f t="shared" si="25"/>
-        <v>1.5895949999999999</v>
+        <v>1.5995533333333332</v>
       </c>
       <c r="I201" s="10"/>
       <c r="T201" s="1">
@@ -11120,11 +11128,11 @@
       </c>
       <c r="V201">
         <f>INT(SUM($U$2:U201)/60)</f>
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="W201">
         <f>(SUM($U$2:U201)-60*V201)/100</f>
-        <v>0.56999999999999995</v>
+        <v>0.32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
editing config, fixing relative paths
</commit_message>
<xml_diff>
--- a/data/raw/Running.xlsx
+++ b/data/raw/Running.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\44752\Desktop\git_repos\Running\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27E485D1-AD71-4781-A8D9-C2C0BBA62AE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66CD1002-CAD8-47EE-B32E-B3E5CC78C275}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A2ECB18D-D6A8-48F0-BC89-850EAC9BB528}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="263">
   <si>
     <t>Date</t>
   </si>
@@ -830,9 +830,6 @@
     <t>5 hr 53.12</t>
   </si>
   <si>
-    <t>23/05/20222</t>
-  </si>
-  <si>
     <t>Tenerife, brutal and savage but completed it mate!</t>
   </si>
   <si>
@@ -1401,8 +1398,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AD3663A-1B36-42F8-92D9-0C097A8D0EBA}">
   <dimension ref="A1:W417"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A342" zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
-      <selection activeCell="H352" sqref="H352"/>
+    <sheetView tabSelected="1" topLeftCell="A350" zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
+      <selection activeCell="F359" sqref="F359"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25.8" outlineLevelCol="1" x14ac:dyDescent="0.5"/>
@@ -16740,8 +16737,8 @@
       </c>
     </row>
     <row r="349" spans="1:21" x14ac:dyDescent="0.5">
-      <c r="A349" s="37" t="s">
-        <v>261</v>
+      <c r="A349" s="37">
+        <v>44704</v>
       </c>
       <c r="B349" s="2" t="s">
         <v>255</v>
@@ -17120,29 +17117,37 @@
       </c>
     </row>
     <row r="359" spans="1:21" x14ac:dyDescent="0.5">
-      <c r="A359" s="9"/>
-      <c r="B359" s="2"/>
-      <c r="C359" s="2"/>
-      <c r="D359" s="5"/>
+      <c r="A359" s="31">
+        <v>44732</v>
+      </c>
+      <c r="B359" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="C359" s="2">
+        <v>3500</v>
+      </c>
+      <c r="D359" s="5">
+        <v>36</v>
+      </c>
       <c r="E359" s="2">
         <f>SUM($C$2:C359)</f>
-        <v>2884905</v>
+        <v>2888405</v>
       </c>
       <c r="F359" s="5">
         <f>SUM($T$2:T359) + V359 + W359</f>
-        <v>17384</v>
+        <v>17420</v>
       </c>
       <c r="G359" s="5">
         <f t="shared" si="38"/>
-        <v>289.73333333333335</v>
+        <v>290.33333333333331</v>
       </c>
       <c r="H359" s="9">
         <f t="shared" si="39"/>
-        <v>2.8973333333333335</v>
+        <v>2.9033333333333333</v>
       </c>
       <c r="T359" s="1">
         <f t="shared" si="40"/>
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="U359" s="1">
         <f t="shared" si="41"/>
@@ -17156,19 +17161,19 @@
       <c r="D360" s="5"/>
       <c r="E360" s="2">
         <f>SUM($C$2:C360)</f>
-        <v>2884905</v>
+        <v>2888405</v>
       </c>
       <c r="F360" s="5">
         <f>SUM($T$2:T360) + V360 + W360</f>
-        <v>17384</v>
+        <v>17420</v>
       </c>
       <c r="G360" s="5">
         <f t="shared" si="38"/>
-        <v>289.73333333333335</v>
+        <v>290.33333333333331</v>
       </c>
       <c r="H360" s="9">
         <f t="shared" si="39"/>
-        <v>2.8973333333333335</v>
+        <v>2.9033333333333333</v>
       </c>
       <c r="T360" s="1">
         <f t="shared" si="40"/>
@@ -17186,19 +17191,19 @@
       <c r="D361" s="5"/>
       <c r="E361" s="2">
         <f>SUM($C$2:C361)</f>
-        <v>2884905</v>
+        <v>2888405</v>
       </c>
       <c r="F361" s="5">
         <f>SUM($T$2:T361) + V361 + W361</f>
-        <v>17384</v>
+        <v>17420</v>
       </c>
       <c r="G361" s="5">
         <f t="shared" si="38"/>
-        <v>289.73333333333335</v>
+        <v>290.33333333333331</v>
       </c>
       <c r="H361" s="9">
         <f t="shared" si="39"/>
-        <v>2.8973333333333335</v>
+        <v>2.9033333333333333</v>
       </c>
       <c r="T361" s="1">
         <f t="shared" si="40"/>
@@ -17216,19 +17221,19 @@
       <c r="D362" s="5"/>
       <c r="E362" s="2">
         <f>SUM($C$2:C362)</f>
-        <v>2884905</v>
+        <v>2888405</v>
       </c>
       <c r="F362" s="5">
         <f>SUM($T$2:T362) + V362 + W362</f>
-        <v>17384</v>
+        <v>17420</v>
       </c>
       <c r="G362" s="5">
         <f t="shared" si="38"/>
-        <v>289.73333333333335</v>
+        <v>290.33333333333331</v>
       </c>
       <c r="H362" s="9">
         <f t="shared" si="39"/>
-        <v>2.8973333333333335</v>
+        <v>2.9033333333333333</v>
       </c>
       <c r="T362" s="1">
         <f t="shared" si="40"/>
@@ -17246,19 +17251,19 @@
       <c r="D363" s="5"/>
       <c r="E363" s="2">
         <f>SUM($C$2:C363)</f>
-        <v>2884905</v>
+        <v>2888405</v>
       </c>
       <c r="F363" s="5">
         <f>SUM($T$2:T363) + V363 + W363</f>
-        <v>17384</v>
+        <v>17420</v>
       </c>
       <c r="G363" s="5">
         <f t="shared" si="38"/>
-        <v>289.73333333333335</v>
+        <v>290.33333333333331</v>
       </c>
       <c r="H363" s="9">
         <f t="shared" si="39"/>
-        <v>2.8973333333333335</v>
+        <v>2.9033333333333333</v>
       </c>
       <c r="T363" s="1">
         <f t="shared" si="40"/>
@@ -17276,19 +17281,19 @@
       <c r="D364" s="5"/>
       <c r="E364" s="2">
         <f>SUM($C$2:C364)</f>
-        <v>2884905</v>
+        <v>2888405</v>
       </c>
       <c r="F364" s="5">
         <f>SUM($T$2:T364) + V364 + W364</f>
-        <v>17384</v>
+        <v>17420</v>
       </c>
       <c r="G364" s="5">
         <f t="shared" si="38"/>
-        <v>289.73333333333335</v>
+        <v>290.33333333333331</v>
       </c>
       <c r="H364" s="9">
         <f t="shared" si="39"/>
-        <v>2.8973333333333335</v>
+        <v>2.9033333333333333</v>
       </c>
       <c r="T364" s="1">
         <f t="shared" si="40"/>
@@ -17306,19 +17311,19 @@
       <c r="D365" s="5"/>
       <c r="E365" s="2">
         <f>SUM($C$2:C365)</f>
-        <v>2884905</v>
+        <v>2888405</v>
       </c>
       <c r="F365" s="5">
         <f>SUM($T$2:T365) + V365 + W365</f>
-        <v>17384</v>
+        <v>17420</v>
       </c>
       <c r="G365" s="5">
         <f t="shared" si="38"/>
-        <v>289.73333333333335</v>
+        <v>290.33333333333331</v>
       </c>
       <c r="H365" s="9">
         <f t="shared" si="39"/>
-        <v>2.8973333333333335</v>
+        <v>2.9033333333333333</v>
       </c>
       <c r="T365" s="1">
         <f t="shared" si="40"/>
@@ -17336,19 +17341,19 @@
       <c r="D366" s="5"/>
       <c r="E366" s="2">
         <f>SUM($C$2:C366)</f>
-        <v>2884905</v>
+        <v>2888405</v>
       </c>
       <c r="F366" s="5">
         <f>SUM($T$2:T366) + V366 + W366</f>
-        <v>17384</v>
+        <v>17420</v>
       </c>
       <c r="G366" s="5">
         <f t="shared" si="38"/>
-        <v>289.73333333333335</v>
+        <v>290.33333333333331</v>
       </c>
       <c r="H366" s="9">
         <f t="shared" si="39"/>
-        <v>2.8973333333333335</v>
+        <v>2.9033333333333333</v>
       </c>
       <c r="T366" s="1">
         <f t="shared" si="40"/>
@@ -17366,19 +17371,19 @@
       <c r="D367" s="5"/>
       <c r="E367" s="2">
         <f>SUM($C$2:C367)</f>
-        <v>2884905</v>
+        <v>2888405</v>
       </c>
       <c r="F367" s="5">
         <f>SUM($T$2:T367) + V367 + W367</f>
-        <v>17384</v>
+        <v>17420</v>
       </c>
       <c r="G367" s="5">
         <f t="shared" ref="G367:G416" si="42">F367/60</f>
-        <v>289.73333333333335</v>
+        <v>290.33333333333331</v>
       </c>
       <c r="H367" s="9">
         <f t="shared" ref="H367:H416" si="43">(F367/600000)*100</f>
-        <v>2.8973333333333335</v>
+        <v>2.9033333333333333</v>
       </c>
       <c r="T367" s="1">
         <f t="shared" si="40"/>
@@ -17396,19 +17401,19 @@
       <c r="D368" s="5"/>
       <c r="E368" s="2">
         <f>SUM($C$2:C368)</f>
-        <v>2884905</v>
+        <v>2888405</v>
       </c>
       <c r="F368" s="5">
         <f>SUM($T$2:T368) + V368 + W368</f>
-        <v>17384</v>
+        <v>17420</v>
       </c>
       <c r="G368" s="5">
         <f t="shared" si="42"/>
-        <v>289.73333333333335</v>
+        <v>290.33333333333331</v>
       </c>
       <c r="H368" s="9">
         <f t="shared" si="43"/>
-        <v>2.8973333333333335</v>
+        <v>2.9033333333333333</v>
       </c>
       <c r="T368" s="1">
         <f t="shared" si="40"/>
@@ -17426,19 +17431,19 @@
       <c r="D369" s="5"/>
       <c r="E369" s="2">
         <f>SUM($C$2:C369)</f>
-        <v>2884905</v>
+        <v>2888405</v>
       </c>
       <c r="F369" s="5">
         <f>SUM($T$2:T369) + V369 + W369</f>
-        <v>17384</v>
+        <v>17420</v>
       </c>
       <c r="G369" s="5">
         <f t="shared" si="42"/>
-        <v>289.73333333333335</v>
+        <v>290.33333333333331</v>
       </c>
       <c r="H369" s="9">
         <f t="shared" si="43"/>
-        <v>2.8973333333333335</v>
+        <v>2.9033333333333333</v>
       </c>
       <c r="T369" s="1">
         <f t="shared" si="40"/>
@@ -17456,19 +17461,19 @@
       <c r="D370" s="5"/>
       <c r="E370" s="2">
         <f>SUM($C$2:C370)</f>
-        <v>2884905</v>
+        <v>2888405</v>
       </c>
       <c r="F370" s="5">
         <f>SUM($T$2:T370) + V370 + W370</f>
-        <v>17384</v>
+        <v>17420</v>
       </c>
       <c r="G370" s="5">
         <f t="shared" si="42"/>
-        <v>289.73333333333335</v>
+        <v>290.33333333333331</v>
       </c>
       <c r="H370" s="9">
         <f t="shared" si="43"/>
-        <v>2.8973333333333335</v>
+        <v>2.9033333333333333</v>
       </c>
       <c r="T370" s="1">
         <f t="shared" si="40"/>
@@ -17486,19 +17491,19 @@
       <c r="D371" s="5"/>
       <c r="E371" s="2">
         <f>SUM($C$2:C371)</f>
-        <v>2884905</v>
+        <v>2888405</v>
       </c>
       <c r="F371" s="5">
         <f>SUM($T$2:T371) + V371 + W371</f>
-        <v>17384</v>
+        <v>17420</v>
       </c>
       <c r="G371" s="5">
         <f t="shared" si="42"/>
-        <v>289.73333333333335</v>
+        <v>290.33333333333331</v>
       </c>
       <c r="H371" s="9">
         <f t="shared" si="43"/>
-        <v>2.8973333333333335</v>
+        <v>2.9033333333333333</v>
       </c>
       <c r="T371" s="1">
         <f t="shared" si="40"/>
@@ -17516,19 +17521,19 @@
       <c r="D372" s="5"/>
       <c r="E372" s="2">
         <f>SUM($C$2:C372)</f>
-        <v>2884905</v>
+        <v>2888405</v>
       </c>
       <c r="F372" s="5">
         <f>SUM($T$2:T372) + V372 + W372</f>
-        <v>17384</v>
+        <v>17420</v>
       </c>
       <c r="G372" s="5">
         <f t="shared" si="42"/>
-        <v>289.73333333333335</v>
+        <v>290.33333333333331</v>
       </c>
       <c r="H372" s="9">
         <f t="shared" si="43"/>
-        <v>2.8973333333333335</v>
+        <v>2.9033333333333333</v>
       </c>
       <c r="T372" s="1">
         <f t="shared" si="40"/>
@@ -17546,19 +17551,19 @@
       <c r="D373" s="5"/>
       <c r="E373" s="2">
         <f>SUM($C$2:C373)</f>
-        <v>2884905</v>
+        <v>2888405</v>
       </c>
       <c r="F373" s="5">
         <f>SUM($T$2:T373) + V373 + W373</f>
-        <v>17384</v>
+        <v>17420</v>
       </c>
       <c r="G373" s="5">
         <f t="shared" si="42"/>
-        <v>289.73333333333335</v>
+        <v>290.33333333333331</v>
       </c>
       <c r="H373" s="9">
         <f t="shared" si="43"/>
-        <v>2.8973333333333335</v>
+        <v>2.9033333333333333</v>
       </c>
       <c r="T373" s="1">
         <f t="shared" ref="T373:T416" si="44">INT(D373)</f>
@@ -17576,19 +17581,19 @@
       <c r="D374" s="5"/>
       <c r="E374" s="2">
         <f>SUM($C$2:C374)</f>
-        <v>2884905</v>
+        <v>2888405</v>
       </c>
       <c r="F374" s="5">
         <f>SUM($T$2:T374) + V374 + W374</f>
-        <v>17384</v>
+        <v>17420</v>
       </c>
       <c r="G374" s="5">
         <f t="shared" si="42"/>
-        <v>289.73333333333335</v>
+        <v>290.33333333333331</v>
       </c>
       <c r="H374" s="9">
         <f t="shared" si="43"/>
-        <v>2.8973333333333335</v>
+        <v>2.9033333333333333</v>
       </c>
       <c r="T374" s="1">
         <f t="shared" si="44"/>
@@ -17606,19 +17611,19 @@
       <c r="D375" s="5"/>
       <c r="E375" s="2">
         <f>SUM($C$2:C375)</f>
-        <v>2884905</v>
+        <v>2888405</v>
       </c>
       <c r="F375" s="5">
         <f>SUM($T$2:T375) + V375 + W375</f>
-        <v>17384</v>
+        <v>17420</v>
       </c>
       <c r="G375" s="5">
         <f t="shared" si="42"/>
-        <v>289.73333333333335</v>
+        <v>290.33333333333331</v>
       </c>
       <c r="H375" s="9">
         <f t="shared" si="43"/>
-        <v>2.8973333333333335</v>
+        <v>2.9033333333333333</v>
       </c>
       <c r="T375" s="1">
         <f t="shared" si="44"/>
@@ -17636,19 +17641,19 @@
       <c r="D376" s="5"/>
       <c r="E376" s="2">
         <f>SUM($C$2:C376)</f>
-        <v>2884905</v>
+        <v>2888405</v>
       </c>
       <c r="F376" s="5">
         <f>SUM($T$2:T376) + V376 + W376</f>
-        <v>17384</v>
+        <v>17420</v>
       </c>
       <c r="G376" s="5">
         <f t="shared" si="42"/>
-        <v>289.73333333333335</v>
+        <v>290.33333333333331</v>
       </c>
       <c r="H376" s="9">
         <f t="shared" si="43"/>
-        <v>2.8973333333333335</v>
+        <v>2.9033333333333333</v>
       </c>
       <c r="T376" s="1">
         <f t="shared" si="44"/>
@@ -17666,19 +17671,19 @@
       <c r="D377" s="5"/>
       <c r="E377" s="2">
         <f>SUM($C$2:C377)</f>
-        <v>2884905</v>
+        <v>2888405</v>
       </c>
       <c r="F377" s="5">
         <f>SUM($T$2:T377) + V377 + W377</f>
-        <v>17384</v>
+        <v>17420</v>
       </c>
       <c r="G377" s="5">
         <f t="shared" si="42"/>
-        <v>289.73333333333335</v>
+        <v>290.33333333333331</v>
       </c>
       <c r="H377" s="9">
         <f t="shared" si="43"/>
-        <v>2.8973333333333335</v>
+        <v>2.9033333333333333</v>
       </c>
       <c r="T377" s="1">
         <f t="shared" si="44"/>
@@ -17696,19 +17701,19 @@
       <c r="D378" s="5"/>
       <c r="E378" s="2">
         <f>SUM($C$2:C378)</f>
-        <v>2884905</v>
+        <v>2888405</v>
       </c>
       <c r="F378" s="5">
         <f>SUM($T$2:T378) + V378 + W378</f>
-        <v>17384</v>
+        <v>17420</v>
       </c>
       <c r="G378" s="5">
         <f t="shared" si="42"/>
-        <v>289.73333333333335</v>
+        <v>290.33333333333331</v>
       </c>
       <c r="H378" s="9">
         <f t="shared" si="43"/>
-        <v>2.8973333333333335</v>
+        <v>2.9033333333333333</v>
       </c>
       <c r="T378" s="1">
         <f t="shared" si="44"/>
@@ -17726,19 +17731,19 @@
       <c r="D379" s="5"/>
       <c r="E379" s="2">
         <f>SUM($C$2:C379)</f>
-        <v>2884905</v>
+        <v>2888405</v>
       </c>
       <c r="F379" s="5">
         <f>SUM($T$2:T379) + V379 + W379</f>
-        <v>17384</v>
+        <v>17420</v>
       </c>
       <c r="G379" s="5">
         <f t="shared" si="42"/>
-        <v>289.73333333333335</v>
+        <v>290.33333333333331</v>
       </c>
       <c r="H379" s="9">
         <f t="shared" si="43"/>
-        <v>2.8973333333333335</v>
+        <v>2.9033333333333333</v>
       </c>
       <c r="T379" s="1">
         <f t="shared" si="44"/>
@@ -17756,19 +17761,19 @@
       <c r="D380" s="5"/>
       <c r="E380" s="2">
         <f>SUM($C$2:C380)</f>
-        <v>2884905</v>
+        <v>2888405</v>
       </c>
       <c r="F380" s="5">
         <f>SUM($T$2:T380) + V380 + W380</f>
-        <v>17384</v>
+        <v>17420</v>
       </c>
       <c r="G380" s="5">
         <f t="shared" si="42"/>
-        <v>289.73333333333335</v>
+        <v>290.33333333333331</v>
       </c>
       <c r="H380" s="9">
         <f t="shared" si="43"/>
-        <v>2.8973333333333335</v>
+        <v>2.9033333333333333</v>
       </c>
       <c r="T380" s="1">
         <f t="shared" si="44"/>
@@ -17786,19 +17791,19 @@
       <c r="D381" s="5"/>
       <c r="E381" s="2">
         <f>SUM($C$2:C381)</f>
-        <v>2884905</v>
+        <v>2888405</v>
       </c>
       <c r="F381" s="5">
         <f>SUM($T$2:T381) + V381 + W381</f>
-        <v>17384</v>
+        <v>17420</v>
       </c>
       <c r="G381" s="5">
         <f t="shared" si="42"/>
-        <v>289.73333333333335</v>
+        <v>290.33333333333331</v>
       </c>
       <c r="H381" s="9">
         <f t="shared" si="43"/>
-        <v>2.8973333333333335</v>
+        <v>2.9033333333333333</v>
       </c>
       <c r="T381" s="1">
         <f t="shared" si="44"/>
@@ -17816,19 +17821,19 @@
       <c r="D382" s="5"/>
       <c r="E382" s="2">
         <f>SUM($C$2:C382)</f>
-        <v>2884905</v>
+        <v>2888405</v>
       </c>
       <c r="F382" s="5">
         <f>SUM($T$2:T382) + V382 + W382</f>
-        <v>17384</v>
+        <v>17420</v>
       </c>
       <c r="G382" s="5">
         <f t="shared" si="42"/>
-        <v>289.73333333333335</v>
+        <v>290.33333333333331</v>
       </c>
       <c r="H382" s="9">
         <f t="shared" si="43"/>
-        <v>2.8973333333333335</v>
+        <v>2.9033333333333333</v>
       </c>
       <c r="T382" s="1">
         <f t="shared" si="44"/>
@@ -17846,19 +17851,19 @@
       <c r="D383" s="5"/>
       <c r="E383" s="2">
         <f>SUM($C$2:C383)</f>
-        <v>2884905</v>
+        <v>2888405</v>
       </c>
       <c r="F383" s="5">
         <f>SUM($T$2:T383) + V383 + W383</f>
-        <v>17384</v>
+        <v>17420</v>
       </c>
       <c r="G383" s="5">
         <f t="shared" si="42"/>
-        <v>289.73333333333335</v>
+        <v>290.33333333333331</v>
       </c>
       <c r="H383" s="9">
         <f t="shared" si="43"/>
-        <v>2.8973333333333335</v>
+        <v>2.9033333333333333</v>
       </c>
       <c r="T383" s="1">
         <f t="shared" si="44"/>
@@ -17876,19 +17881,19 @@
       <c r="D384" s="5"/>
       <c r="E384" s="2">
         <f>SUM($C$2:C384)</f>
-        <v>2884905</v>
+        <v>2888405</v>
       </c>
       <c r="F384" s="5">
         <f>SUM($T$2:T384) + V384 + W384</f>
-        <v>17384</v>
+        <v>17420</v>
       </c>
       <c r="G384" s="5">
         <f t="shared" si="42"/>
-        <v>289.73333333333335</v>
+        <v>290.33333333333331</v>
       </c>
       <c r="H384" s="9">
         <f t="shared" si="43"/>
-        <v>2.8973333333333335</v>
+        <v>2.9033333333333333</v>
       </c>
       <c r="T384" s="1">
         <f t="shared" si="44"/>
@@ -17906,19 +17911,19 @@
       <c r="D385" s="5"/>
       <c r="E385" s="2">
         <f>SUM($C$2:C385)</f>
-        <v>2884905</v>
+        <v>2888405</v>
       </c>
       <c r="F385" s="5">
         <f>SUM($T$2:T385) + V385 + W385</f>
-        <v>17384</v>
+        <v>17420</v>
       </c>
       <c r="G385" s="5">
         <f t="shared" si="42"/>
-        <v>289.73333333333335</v>
+        <v>290.33333333333331</v>
       </c>
       <c r="H385" s="9">
         <f t="shared" si="43"/>
-        <v>2.8973333333333335</v>
+        <v>2.9033333333333333</v>
       </c>
       <c r="T385" s="1">
         <f t="shared" si="44"/>
@@ -17936,19 +17941,19 @@
       <c r="D386" s="5"/>
       <c r="E386" s="2">
         <f>SUM($C$2:C386)</f>
-        <v>2884905</v>
+        <v>2888405</v>
       </c>
       <c r="F386" s="5">
         <f>SUM($T$2:T386) + V386 + W386</f>
-        <v>17384</v>
+        <v>17420</v>
       </c>
       <c r="G386" s="5">
         <f t="shared" si="42"/>
-        <v>289.73333333333335</v>
+        <v>290.33333333333331</v>
       </c>
       <c r="H386" s="9">
         <f t="shared" si="43"/>
-        <v>2.8973333333333335</v>
+        <v>2.9033333333333333</v>
       </c>
       <c r="T386" s="1">
         <f t="shared" si="44"/>
@@ -17966,19 +17971,19 @@
       <c r="D387" s="5"/>
       <c r="E387" s="2">
         <f>SUM($C$2:C387)</f>
-        <v>2884905</v>
+        <v>2888405</v>
       </c>
       <c r="F387" s="5">
         <f>SUM($T$2:T387) + V387 + W387</f>
-        <v>17384</v>
+        <v>17420</v>
       </c>
       <c r="G387" s="5">
         <f t="shared" si="42"/>
-        <v>289.73333333333335</v>
+        <v>290.33333333333331</v>
       </c>
       <c r="H387" s="9">
         <f t="shared" si="43"/>
-        <v>2.8973333333333335</v>
+        <v>2.9033333333333333</v>
       </c>
       <c r="T387" s="1">
         <f t="shared" si="44"/>
@@ -17996,19 +18001,19 @@
       <c r="D388" s="5"/>
       <c r="E388" s="2">
         <f>SUM($C$2:C388)</f>
-        <v>2884905</v>
+        <v>2888405</v>
       </c>
       <c r="F388" s="5">
         <f>SUM($T$2:T388) + V388 + W388</f>
-        <v>17384</v>
+        <v>17420</v>
       </c>
       <c r="G388" s="5">
         <f t="shared" si="42"/>
-        <v>289.73333333333335</v>
+        <v>290.33333333333331</v>
       </c>
       <c r="H388" s="9">
         <f t="shared" si="43"/>
-        <v>2.8973333333333335</v>
+        <v>2.9033333333333333</v>
       </c>
       <c r="T388" s="1">
         <f t="shared" si="44"/>
@@ -18026,19 +18031,19 @@
       <c r="D389" s="5"/>
       <c r="E389" s="2">
         <f>SUM($C$2:C389)</f>
-        <v>2884905</v>
+        <v>2888405</v>
       </c>
       <c r="F389" s="5">
         <f>SUM($T$2:T389) + V389 + W389</f>
-        <v>17384</v>
+        <v>17420</v>
       </c>
       <c r="G389" s="5">
         <f t="shared" si="42"/>
-        <v>289.73333333333335</v>
+        <v>290.33333333333331</v>
       </c>
       <c r="H389" s="9">
         <f t="shared" si="43"/>
-        <v>2.8973333333333335</v>
+        <v>2.9033333333333333</v>
       </c>
       <c r="T389" s="1">
         <f t="shared" si="44"/>
@@ -18056,19 +18061,19 @@
       <c r="D390" s="5"/>
       <c r="E390" s="2">
         <f>SUM($C$2:C390)</f>
-        <v>2884905</v>
+        <v>2888405</v>
       </c>
       <c r="F390" s="5">
         <f>SUM($T$2:T390) + V390 + W390</f>
-        <v>17384</v>
+        <v>17420</v>
       </c>
       <c r="G390" s="5">
         <f t="shared" si="42"/>
-        <v>289.73333333333335</v>
+        <v>290.33333333333331</v>
       </c>
       <c r="H390" s="9">
         <f t="shared" si="43"/>
-        <v>2.8973333333333335</v>
+        <v>2.9033333333333333</v>
       </c>
       <c r="T390" s="1">
         <f t="shared" si="44"/>
@@ -18086,19 +18091,19 @@
       <c r="D391" s="5"/>
       <c r="E391" s="2">
         <f>SUM($C$2:C391)</f>
-        <v>2884905</v>
+        <v>2888405</v>
       </c>
       <c r="F391" s="5">
         <f>SUM($T$2:T391) + V391 + W391</f>
-        <v>17384</v>
+        <v>17420</v>
       </c>
       <c r="G391" s="5">
         <f t="shared" si="42"/>
-        <v>289.73333333333335</v>
+        <v>290.33333333333331</v>
       </c>
       <c r="H391" s="9">
         <f t="shared" si="43"/>
-        <v>2.8973333333333335</v>
+        <v>2.9033333333333333</v>
       </c>
       <c r="T391" s="1">
         <f t="shared" si="44"/>
@@ -18116,19 +18121,19 @@
       <c r="D392" s="5"/>
       <c r="E392" s="2">
         <f>SUM($C$2:C392)</f>
-        <v>2884905</v>
+        <v>2888405</v>
       </c>
       <c r="F392" s="5">
         <f>SUM($T$2:T392) + V392 + W392</f>
-        <v>17384</v>
+        <v>17420</v>
       </c>
       <c r="G392" s="5">
         <f t="shared" si="42"/>
-        <v>289.73333333333335</v>
+        <v>290.33333333333331</v>
       </c>
       <c r="H392" s="9">
         <f t="shared" si="43"/>
-        <v>2.8973333333333335</v>
+        <v>2.9033333333333333</v>
       </c>
       <c r="T392" s="1">
         <f t="shared" si="44"/>
@@ -18146,19 +18151,19 @@
       <c r="D393" s="5"/>
       <c r="E393" s="2">
         <f>SUM($C$2:C393)</f>
-        <v>2884905</v>
+        <v>2888405</v>
       </c>
       <c r="F393" s="5">
         <f>SUM($T$2:T393) + V393 + W393</f>
-        <v>17384</v>
+        <v>17420</v>
       </c>
       <c r="G393" s="5">
         <f t="shared" si="42"/>
-        <v>289.73333333333335</v>
+        <v>290.33333333333331</v>
       </c>
       <c r="H393" s="9">
         <f t="shared" si="43"/>
-        <v>2.8973333333333335</v>
+        <v>2.9033333333333333</v>
       </c>
       <c r="T393" s="1">
         <f t="shared" si="44"/>
@@ -18176,19 +18181,19 @@
       <c r="D394" s="5"/>
       <c r="E394" s="2">
         <f>SUM($C$2:C394)</f>
-        <v>2884905</v>
+        <v>2888405</v>
       </c>
       <c r="F394" s="5">
         <f>SUM($T$2:T394) + V394 + W394</f>
-        <v>17384</v>
+        <v>17420</v>
       </c>
       <c r="G394" s="5">
         <f t="shared" si="42"/>
-        <v>289.73333333333335</v>
+        <v>290.33333333333331</v>
       </c>
       <c r="H394" s="9">
         <f t="shared" si="43"/>
-        <v>2.8973333333333335</v>
+        <v>2.9033333333333333</v>
       </c>
       <c r="T394" s="1">
         <f t="shared" si="44"/>
@@ -18206,19 +18211,19 @@
       <c r="D395" s="5"/>
       <c r="E395" s="2">
         <f>SUM($C$2:C395)</f>
-        <v>2884905</v>
+        <v>2888405</v>
       </c>
       <c r="F395" s="5">
         <f>SUM($T$2:T395) + V395 + W395</f>
-        <v>17384</v>
+        <v>17420</v>
       </c>
       <c r="G395" s="5">
         <f t="shared" si="42"/>
-        <v>289.73333333333335</v>
+        <v>290.33333333333331</v>
       </c>
       <c r="H395" s="9">
         <f t="shared" si="43"/>
-        <v>2.8973333333333335</v>
+        <v>2.9033333333333333</v>
       </c>
       <c r="T395" s="1">
         <f t="shared" si="44"/>
@@ -18236,19 +18241,19 @@
       <c r="D396" s="5"/>
       <c r="E396" s="2">
         <f>SUM($C$2:C396)</f>
-        <v>2884905</v>
+        <v>2888405</v>
       </c>
       <c r="F396" s="5">
         <f>SUM($T$2:T396) + V396 + W396</f>
-        <v>17384</v>
+        <v>17420</v>
       </c>
       <c r="G396" s="5">
         <f t="shared" si="42"/>
-        <v>289.73333333333335</v>
+        <v>290.33333333333331</v>
       </c>
       <c r="H396" s="9">
         <f t="shared" si="43"/>
-        <v>2.8973333333333335</v>
+        <v>2.9033333333333333</v>
       </c>
       <c r="T396" s="1">
         <f t="shared" si="44"/>
@@ -18266,19 +18271,19 @@
       <c r="D397" s="5"/>
       <c r="E397" s="2">
         <f>SUM($C$2:C397)</f>
-        <v>2884905</v>
+        <v>2888405</v>
       </c>
       <c r="F397" s="5">
         <f>SUM($T$2:T397) + V397 + W397</f>
-        <v>17384</v>
+        <v>17420</v>
       </c>
       <c r="G397" s="5">
         <f t="shared" si="42"/>
-        <v>289.73333333333335</v>
+        <v>290.33333333333331</v>
       </c>
       <c r="H397" s="9">
         <f t="shared" si="43"/>
-        <v>2.8973333333333335</v>
+        <v>2.9033333333333333</v>
       </c>
       <c r="T397" s="1">
         <f t="shared" si="44"/>
@@ -18296,19 +18301,19 @@
       <c r="D398" s="5"/>
       <c r="E398" s="2">
         <f>SUM($C$2:C398)</f>
-        <v>2884905</v>
+        <v>2888405</v>
       </c>
       <c r="F398" s="5">
         <f>SUM($T$2:T398) + V398 + W398</f>
-        <v>17384</v>
+        <v>17420</v>
       </c>
       <c r="G398" s="5">
         <f t="shared" si="42"/>
-        <v>289.73333333333335</v>
+        <v>290.33333333333331</v>
       </c>
       <c r="H398" s="9">
         <f t="shared" si="43"/>
-        <v>2.8973333333333335</v>
+        <v>2.9033333333333333</v>
       </c>
       <c r="T398" s="1">
         <f t="shared" si="44"/>
@@ -18326,19 +18331,19 @@
       <c r="D399" s="5"/>
       <c r="E399" s="2">
         <f>SUM($C$2:C399)</f>
-        <v>2884905</v>
+        <v>2888405</v>
       </c>
       <c r="F399" s="5">
         <f>SUM($T$2:T399) + V399 + W399</f>
-        <v>17384</v>
+        <v>17420</v>
       </c>
       <c r="G399" s="5">
         <f t="shared" si="42"/>
-        <v>289.73333333333335</v>
+        <v>290.33333333333331</v>
       </c>
       <c r="H399" s="9">
         <f t="shared" si="43"/>
-        <v>2.8973333333333335</v>
+        <v>2.9033333333333333</v>
       </c>
       <c r="T399" s="1">
         <f t="shared" si="44"/>
@@ -18356,19 +18361,19 @@
       <c r="D400" s="5"/>
       <c r="E400" s="2">
         <f>SUM($C$2:C400)</f>
-        <v>2884905</v>
+        <v>2888405</v>
       </c>
       <c r="F400" s="5">
         <f>SUM($T$2:T400) + V400 + W400</f>
-        <v>17384</v>
+        <v>17420</v>
       </c>
       <c r="G400" s="5">
         <f t="shared" si="42"/>
-        <v>289.73333333333335</v>
+        <v>290.33333333333331</v>
       </c>
       <c r="H400" s="9">
         <f t="shared" si="43"/>
-        <v>2.8973333333333335</v>
+        <v>2.9033333333333333</v>
       </c>
       <c r="T400" s="1">
         <f t="shared" si="44"/>
@@ -18386,19 +18391,19 @@
       <c r="D401" s="5"/>
       <c r="E401" s="2">
         <f>SUM($C$2:C401)</f>
-        <v>2884905</v>
+        <v>2888405</v>
       </c>
       <c r="F401" s="5">
         <f>SUM($T$2:T401) + V401 + W401</f>
-        <v>17384</v>
+        <v>17420</v>
       </c>
       <c r="G401" s="5">
         <f t="shared" si="42"/>
-        <v>289.73333333333335</v>
+        <v>290.33333333333331</v>
       </c>
       <c r="H401" s="9">
         <f t="shared" si="43"/>
-        <v>2.8973333333333335</v>
+        <v>2.9033333333333333</v>
       </c>
       <c r="T401" s="1">
         <f t="shared" si="44"/>
@@ -18416,19 +18421,19 @@
       <c r="D402" s="5"/>
       <c r="E402" s="2">
         <f>SUM($C$2:C402)</f>
-        <v>2884905</v>
+        <v>2888405</v>
       </c>
       <c r="F402" s="5">
         <f>SUM($T$2:T402) + V402 + W402</f>
-        <v>17384</v>
+        <v>17420</v>
       </c>
       <c r="G402" s="5">
         <f t="shared" si="42"/>
-        <v>289.73333333333335</v>
+        <v>290.33333333333331</v>
       </c>
       <c r="H402" s="9">
         <f t="shared" si="43"/>
-        <v>2.8973333333333335</v>
+        <v>2.9033333333333333</v>
       </c>
       <c r="T402" s="1">
         <f t="shared" si="44"/>
@@ -18446,19 +18451,19 @@
       <c r="D403" s="5"/>
       <c r="E403" s="2">
         <f>SUM($C$2:C403)</f>
-        <v>2884905</v>
+        <v>2888405</v>
       </c>
       <c r="F403" s="5">
         <f>SUM($T$2:T403) + V403 + W403</f>
-        <v>17384</v>
+        <v>17420</v>
       </c>
       <c r="G403" s="5">
         <f t="shared" si="42"/>
-        <v>289.73333333333335</v>
+        <v>290.33333333333331</v>
       </c>
       <c r="H403" s="9">
         <f t="shared" si="43"/>
-        <v>2.8973333333333335</v>
+        <v>2.9033333333333333</v>
       </c>
       <c r="T403" s="1">
         <f t="shared" si="44"/>
@@ -18476,19 +18481,19 @@
       <c r="D404" s="5"/>
       <c r="E404" s="2">
         <f>SUM($C$2:C404)</f>
-        <v>2884905</v>
+        <v>2888405</v>
       </c>
       <c r="F404" s="5">
         <f>SUM($T$2:T404) + V404 + W404</f>
-        <v>17384</v>
+        <v>17420</v>
       </c>
       <c r="G404" s="5">
         <f t="shared" si="42"/>
-        <v>289.73333333333335</v>
+        <v>290.33333333333331</v>
       </c>
       <c r="H404" s="9">
         <f t="shared" si="43"/>
-        <v>2.8973333333333335</v>
+        <v>2.9033333333333333</v>
       </c>
       <c r="T404" s="1">
         <f t="shared" si="44"/>
@@ -18506,19 +18511,19 @@
       <c r="D405" s="5"/>
       <c r="E405" s="2">
         <f>SUM($C$2:C405)</f>
-        <v>2884905</v>
+        <v>2888405</v>
       </c>
       <c r="F405" s="5">
         <f>SUM($T$2:T405) + V405 + W405</f>
-        <v>17384</v>
+        <v>17420</v>
       </c>
       <c r="G405" s="5">
         <f t="shared" si="42"/>
-        <v>289.73333333333335</v>
+        <v>290.33333333333331</v>
       </c>
       <c r="H405" s="9">
         <f t="shared" si="43"/>
-        <v>2.8973333333333335</v>
+        <v>2.9033333333333333</v>
       </c>
       <c r="T405" s="1">
         <f t="shared" si="44"/>
@@ -18536,19 +18541,19 @@
       <c r="D406" s="5"/>
       <c r="E406" s="2">
         <f>SUM($C$2:C406)</f>
-        <v>2884905</v>
+        <v>2888405</v>
       </c>
       <c r="F406" s="5">
         <f>SUM($T$2:T406) + V406 + W406</f>
-        <v>17384</v>
+        <v>17420</v>
       </c>
       <c r="G406" s="5">
         <f t="shared" si="42"/>
-        <v>289.73333333333335</v>
+        <v>290.33333333333331</v>
       </c>
       <c r="H406" s="9">
         <f t="shared" si="43"/>
-        <v>2.8973333333333335</v>
+        <v>2.9033333333333333</v>
       </c>
       <c r="T406" s="1">
         <f t="shared" si="44"/>
@@ -18566,19 +18571,19 @@
       <c r="D407" s="5"/>
       <c r="E407" s="2">
         <f>SUM($C$2:C407)</f>
-        <v>2884905</v>
+        <v>2888405</v>
       </c>
       <c r="F407" s="5">
         <f>SUM($T$2:T407) + V407 + W407</f>
-        <v>17384</v>
+        <v>17420</v>
       </c>
       <c r="G407" s="5">
         <f t="shared" si="42"/>
-        <v>289.73333333333335</v>
+        <v>290.33333333333331</v>
       </c>
       <c r="H407" s="9">
         <f t="shared" si="43"/>
-        <v>2.8973333333333335</v>
+        <v>2.9033333333333333</v>
       </c>
       <c r="T407" s="1">
         <f t="shared" si="44"/>
@@ -18596,19 +18601,19 @@
       <c r="D408" s="5"/>
       <c r="E408" s="2">
         <f>SUM($C$2:C408)</f>
-        <v>2884905</v>
+        <v>2888405</v>
       </c>
       <c r="F408" s="5">
         <f>SUM($T$2:T408) + V408 + W408</f>
-        <v>17384</v>
+        <v>17420</v>
       </c>
       <c r="G408" s="5">
         <f t="shared" si="42"/>
-        <v>289.73333333333335</v>
+        <v>290.33333333333331</v>
       </c>
       <c r="H408" s="9">
         <f t="shared" si="43"/>
-        <v>2.8973333333333335</v>
+        <v>2.9033333333333333</v>
       </c>
       <c r="T408" s="1">
         <f t="shared" si="44"/>
@@ -18626,19 +18631,19 @@
       <c r="D409" s="5"/>
       <c r="E409" s="2">
         <f>SUM($C$2:C409)</f>
-        <v>2884905</v>
+        <v>2888405</v>
       </c>
       <c r="F409" s="5">
         <f>SUM($T$2:T409) + V409 + W409</f>
-        <v>17384</v>
+        <v>17420</v>
       </c>
       <c r="G409" s="5">
         <f t="shared" si="42"/>
-        <v>289.73333333333335</v>
+        <v>290.33333333333331</v>
       </c>
       <c r="H409" s="9">
         <f t="shared" si="43"/>
-        <v>2.8973333333333335</v>
+        <v>2.9033333333333333</v>
       </c>
       <c r="T409" s="1">
         <f t="shared" si="44"/>
@@ -18656,19 +18661,19 @@
       <c r="D410" s="5"/>
       <c r="E410" s="2">
         <f>SUM($C$2:C410)</f>
-        <v>2884905</v>
+        <v>2888405</v>
       </c>
       <c r="F410" s="5">
         <f>SUM($T$2:T410) + V410 + W410</f>
-        <v>17384</v>
+        <v>17420</v>
       </c>
       <c r="G410" s="5">
         <f t="shared" si="42"/>
-        <v>289.73333333333335</v>
+        <v>290.33333333333331</v>
       </c>
       <c r="H410" s="9">
         <f t="shared" si="43"/>
-        <v>2.8973333333333335</v>
+        <v>2.9033333333333333</v>
       </c>
       <c r="T410" s="1">
         <f t="shared" si="44"/>
@@ -18686,19 +18691,19 @@
       <c r="D411" s="5"/>
       <c r="E411" s="2">
         <f>SUM($C$2:C411)</f>
-        <v>2884905</v>
+        <v>2888405</v>
       </c>
       <c r="F411" s="5">
         <f>SUM($T$2:T411) + V411 + W411</f>
-        <v>17384</v>
+        <v>17420</v>
       </c>
       <c r="G411" s="5">
         <f t="shared" si="42"/>
-        <v>289.73333333333335</v>
+        <v>290.33333333333331</v>
       </c>
       <c r="H411" s="9">
         <f t="shared" si="43"/>
-        <v>2.8973333333333335</v>
+        <v>2.9033333333333333</v>
       </c>
       <c r="T411" s="1">
         <f t="shared" si="44"/>
@@ -18716,19 +18721,19 @@
       <c r="D412" s="5"/>
       <c r="E412" s="2">
         <f>SUM($C$2:C412)</f>
-        <v>2884905</v>
+        <v>2888405</v>
       </c>
       <c r="F412" s="5">
         <f>SUM($T$2:T412) + V412 + W412</f>
-        <v>17384</v>
+        <v>17420</v>
       </c>
       <c r="G412" s="5">
         <f t="shared" si="42"/>
-        <v>289.73333333333335</v>
+        <v>290.33333333333331</v>
       </c>
       <c r="H412" s="9">
         <f t="shared" si="43"/>
-        <v>2.8973333333333335</v>
+        <v>2.9033333333333333</v>
       </c>
       <c r="T412" s="1">
         <f t="shared" si="44"/>
@@ -18746,19 +18751,19 @@
       <c r="D413" s="5"/>
       <c r="E413" s="2">
         <f>SUM($C$2:C413)</f>
-        <v>2884905</v>
+        <v>2888405</v>
       </c>
       <c r="F413" s="5">
         <f>SUM($T$2:T413) + V413 + W413</f>
-        <v>17384</v>
+        <v>17420</v>
       </c>
       <c r="G413" s="5">
         <f t="shared" si="42"/>
-        <v>289.73333333333335</v>
+        <v>290.33333333333331</v>
       </c>
       <c r="H413" s="9">
         <f t="shared" si="43"/>
-        <v>2.8973333333333335</v>
+        <v>2.9033333333333333</v>
       </c>
       <c r="T413" s="1">
         <f t="shared" si="44"/>
@@ -18776,19 +18781,19 @@
       <c r="D414" s="5"/>
       <c r="E414" s="2">
         <f>SUM($C$2:C414)</f>
-        <v>2884905</v>
+        <v>2888405</v>
       </c>
       <c r="F414" s="5">
         <f>SUM($T$2:T414) + V414 + W414</f>
-        <v>17384</v>
+        <v>17420</v>
       </c>
       <c r="G414" s="5">
         <f t="shared" si="42"/>
-        <v>289.73333333333335</v>
+        <v>290.33333333333331</v>
       </c>
       <c r="H414" s="9">
         <f t="shared" si="43"/>
-        <v>2.8973333333333335</v>
+        <v>2.9033333333333333</v>
       </c>
       <c r="T414" s="1">
         <f t="shared" si="44"/>
@@ -18806,19 +18811,19 @@
       <c r="D415" s="5"/>
       <c r="E415" s="2">
         <f>SUM($C$2:C415)</f>
-        <v>2884905</v>
+        <v>2888405</v>
       </c>
       <c r="F415" s="5">
         <f>SUM($T$2:T415) + V415 + W415</f>
-        <v>17384</v>
+        <v>17420</v>
       </c>
       <c r="G415" s="5">
         <f t="shared" si="42"/>
-        <v>289.73333333333335</v>
+        <v>290.33333333333331</v>
       </c>
       <c r="H415" s="9">
         <f t="shared" si="43"/>
-        <v>2.8973333333333335</v>
+        <v>2.9033333333333333</v>
       </c>
       <c r="T415" s="1">
         <f t="shared" si="44"/>
@@ -18836,19 +18841,19 @@
       <c r="D416" s="5"/>
       <c r="E416" s="2">
         <f>SUM($C$2:C416)</f>
-        <v>2884905</v>
+        <v>2888405</v>
       </c>
       <c r="F416" s="5">
         <f>SUM($T$2:T416) + V416 + W416</f>
-        <v>17384</v>
+        <v>17420</v>
       </c>
       <c r="G416" s="5">
         <f t="shared" si="42"/>
-        <v>289.73333333333335</v>
+        <v>290.33333333333331</v>
       </c>
       <c r="H416" s="9">
         <f t="shared" si="43"/>
-        <v>2.8973333333333335</v>
+        <v>2.9033333333333333</v>
       </c>
       <c r="T416" s="1">
         <f t="shared" si="44"/>
@@ -40602,7 +40607,7 @@
         <v>44716</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -40659,7 +40664,7 @@
         <v>44716</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>